<commit_message>
Implemented use of real car travel times between stations
</commit_message>
<xml_diff>
--- a/data/addresses.xlsx
+++ b/data/addresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28C64A4-7FF4-44DA-8D6E-D89AD4E5C72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B42F1-791B-4B9D-9DEB-EDB7CEC3F93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="15585" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B0D1EE3-07DA-4BB2-A671-24263A9F0D10}"/>
+    <workbookView xWindow="57480" yWindow="15585" windowWidth="29040" windowHeight="15840" xr2:uid="{4B0D1EE3-07DA-4BB2-A671-24263A9F0D10}"/>
   </bookViews>
   <sheets>
     <sheet name="Linking station names" sheetId="1" r:id="rId1"/>
@@ -690,9 +690,6 @@
     <t>Station</t>
   </si>
   <si>
-    <t>Station name in adress list</t>
-  </si>
-  <si>
     <t>Address (automatically determined)</t>
   </si>
   <si>
@@ -760,6 +757,9 @@
   </si>
   <si>
     <t>Stationspark 14, 4461 HK Goes</t>
+  </si>
+  <si>
+    <t>Station name in address list</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C23A643-29F4-469D-948F-B38812878EAE}">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1145,10 +1145,10 @@
         <v>141</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1324,7 +1324,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>_xlfn.XLOOKUP(B16,'Station addresses'!$A$2:$A$1008,'Station addresses'!$B$2:$B$1008,"STATION NOT FOUND IN ADDRESS LIST")</f>
@@ -2180,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D40E918-4E91-4C95-B234-1F9922AFEF3D}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2198,7 @@
         <v>212</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -2315,13 +2315,13 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2401,10 +2401,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -2444,10 +2444,10 @@
         <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2455,10 +2455,10 @@
         <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2562,10 +2562,10 @@
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -2581,10 +2581,10 @@
         <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -2616,10 +2616,10 @@
         <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2691,10 +2691,10 @@
         <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -2718,7 +2718,7 @@
         <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -2901,10 +2901,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2966,42 +2966,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -3012,7 +3012,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>